<commit_message>
updated genbank submission tsv sheet
</commit_message>
<xml_diff>
--- a/GenBank_submission/second_submission/SRA_bioproject_links.xlsx
+++ b/GenBank_submission/second_submission/SRA_bioproject_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwenddolenkettenburg/Desktop/developer/mada-bat-picornavirus/GenBank_submission/second_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1607C758-5788-0245-BFCE-8C9F96EB4E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C60863-7238-654B-9B6E-7928151D8ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29540" yWindow="-1980" windowWidth="12840" windowHeight="19100" xr2:uid="{F5949B09-E751-A24B-8740-6DF68A23678F}"/>
+    <workbookView xWindow="6480" yWindow="740" windowWidth="16420" windowHeight="17340" xr2:uid="{F5949B09-E751-A24B-8740-6DF68A23678F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,105 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
   <si>
-    <t>bioproject_accession</t>
-  </si>
-  <si>
-    <t>biosample_accession</t>
-  </si>
-  <si>
-    <t>SRA_accession</t>
-  </si>
-  <si>
-    <t>ANG22</t>
-  </si>
-  <si>
-    <t>ANG141</t>
-  </si>
-  <si>
-    <t>ANGB110.1</t>
-  </si>
-  <si>
-    <t>ANGB110.2</t>
-  </si>
-  <si>
-    <t>ANGB110.3</t>
-  </si>
-  <si>
-    <t>ANGB121</t>
-  </si>
-  <si>
-    <t>KEL72</t>
-  </si>
-  <si>
-    <t>KEL86</t>
-  </si>
-  <si>
-    <t>KEL148.1</t>
-  </si>
-  <si>
-    <t>KEL148.2</t>
-  </si>
-  <si>
-    <t>KEL168</t>
-  </si>
-  <si>
-    <t>KEL200</t>
-  </si>
-  <si>
-    <t>KEL207</t>
-  </si>
-  <si>
-    <t>KEL273.1</t>
-  </si>
-  <si>
-    <t>KEL273.2</t>
-  </si>
-  <si>
-    <t>KEL275B.1</t>
-  </si>
-  <si>
-    <t>KEL298.1</t>
-  </si>
-  <si>
-    <t>KEL298.2</t>
-  </si>
-  <si>
-    <t>KEL367</t>
-  </si>
-  <si>
-    <t>MIZ219.1</t>
-  </si>
-  <si>
-    <t>MIZ405.1</t>
-  </si>
-  <si>
-    <t>MIZ405.2</t>
-  </si>
-  <si>
-    <t>MIZ405.3</t>
-  </si>
-  <si>
-    <t>MIZ405.4</t>
-  </si>
-  <si>
-    <t>MIZ405.5</t>
-  </si>
-  <si>
-    <t>MIZ405.6</t>
-  </si>
-  <si>
-    <t>MIZ405.7</t>
-  </si>
-  <si>
-    <t>MIZ405.8</t>
-  </si>
-  <si>
-    <t>MIZ405.9</t>
-  </si>
-  <si>
-    <t>Sequence_ID</t>
-  </si>
-  <si>
     <t>SRR24138312</t>
   </si>
   <si>
@@ -237,6 +138,105 @@
   </si>
   <si>
     <t>SAMN41191150</t>
+  </si>
+  <si>
+    <t>Accession</t>
+  </si>
+  <si>
+    <t>PP766449</t>
+  </si>
+  <si>
+    <t>PP766450</t>
+  </si>
+  <si>
+    <t>PP766451</t>
+  </si>
+  <si>
+    <t>PP766452</t>
+  </si>
+  <si>
+    <t>PP766453</t>
+  </si>
+  <si>
+    <t>PP766454</t>
+  </si>
+  <si>
+    <t>PP766455</t>
+  </si>
+  <si>
+    <t>PP766456</t>
+  </si>
+  <si>
+    <t>PP766457</t>
+  </si>
+  <si>
+    <t>PP766458</t>
+  </si>
+  <si>
+    <t>PP766459</t>
+  </si>
+  <si>
+    <t>PP766461</t>
+  </si>
+  <si>
+    <t>PP766460</t>
+  </si>
+  <si>
+    <t>PP766462</t>
+  </si>
+  <si>
+    <t>PP766463</t>
+  </si>
+  <si>
+    <t>PP766464</t>
+  </si>
+  <si>
+    <t>PP766465</t>
+  </si>
+  <si>
+    <t>PP766466</t>
+  </si>
+  <si>
+    <t>PP766467</t>
+  </si>
+  <si>
+    <t>PP766468</t>
+  </si>
+  <si>
+    <t>PP766469</t>
+  </si>
+  <si>
+    <t>PP766470</t>
+  </si>
+  <si>
+    <t>PP766471</t>
+  </si>
+  <si>
+    <t>PP766472</t>
+  </si>
+  <si>
+    <t>PP766473</t>
+  </si>
+  <si>
+    <t>PP766474</t>
+  </si>
+  <si>
+    <t>PP766475</t>
+  </si>
+  <si>
+    <t>PP766476</t>
+  </si>
+  <si>
+    <t>PP766477</t>
+  </si>
+  <si>
+    <t>Bioproject</t>
+  </si>
+  <si>
+    <t>Biosample</t>
+  </si>
+  <si>
+    <t>SRA</t>
   </si>
 </sst>
 </file>
@@ -611,7 +611,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -621,422 +621,422 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>61</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>